<commit_message>
gg typo fix for real
</commit_message>
<xml_diff>
--- a/gary-gygax/checklist.xlsx
+++ b/gary-gygax/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/gary-gygax/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE799106-93FA-B24B-8AF3-BA9EF560E7B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE81606D-AA7E-1942-B897-CE5AAB1F5449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{BB6AF2A8-1098-434F-844D-96BFE025E142}"/>
   </bookViews>
@@ -74,7 +74,7 @@
     <t>role-playing-mastery.jpg</t>
   </si>
   <si>
-    <t>Matser of the Game</t>
+    <t>Master of the Game</t>
   </si>
 </sst>
 </file>

</xml_diff>